<commit_message>
테스트케이스.xlsx  TC-0006,TC-0008,TC-0010 결함 Pass로 수정
</commit_message>
<xml_diff>
--- a/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스.xlsx
+++ b/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eunho\SE2017_4_tuna\doc\4_ 테스트케이스 및 테스트결과보고서\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="11025" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="이력" sheetId="2" r:id="rId1"/>
     <sheet name="테스트케이스" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="240">
   <si>
     <t>TestCase ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,13 +54,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>결함일 경우, Redmine 이슈번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>총 TC 수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -98,21 +86,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>테스트 전에 되어 있어야 하는 것
-예) 로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 테스트 케이스가 검증하고자 하는 것
-예) 입력 기능에 대한 에러 검출</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>테스트 입력값
-예) 소프트웨어공학</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Usecase ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -121,38 +94,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(순차적) 테스트 실행 절차
-예)
-1. XXX를 클릭한다.
-2. 입력값을 넣는다.
-3. 확인을 클릭한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2016. 03. 24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예) 입력 성공 메시지 출력
-     - "성공하였습니다."</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TestCase 이력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>&lt;변경 이력&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Usecase ID
-(테스트 대상 기능)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Testcase 일련번호
-예) TC-0001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1080,21 +1026,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Fail
-빈 공간 선택에 대한 에러 메시지가 출력되지 않음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fail
-항목명 미입력에 대한 에러 메시지가 출력되지않음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fail 
-등록되지 않은 과목 수정 불가에 대한 에러 메시지가 출력되지않음.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2017.06.05</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1144,23 +1075,36 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2017.06.05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TC-0016 결함 Pass로 변경</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>김은호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.06.06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.06.06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0006,TC-0008,TC-0010 
+결함 Pass로 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정화인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1191,14 +1135,6 @@
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -1473,7 +1409,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1488,12 +1424,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1534,16 +1464,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1561,13 +1491,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1876,232 +1806,240 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="2" width="15.625" customWidth="1"/>
-    <col min="3" max="3" width="22.375" customWidth="1"/>
-    <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="1" max="2" width="15.58203125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="41.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D4" s="23" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-    </row>
-    <row r="7" spans="1:4" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="21"/>
-    </row>
-    <row r="8" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+    <row r="1" spans="1:4" ht="39.5">
+      <c r="B1" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="7.5" customHeight="1"/>
+    <row r="3" spans="1:4" ht="6.75" customHeight="1"/>
+    <row r="4" spans="1:4" ht="21">
+      <c r="D4" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="54" customHeight="1"/>
+    <row r="6" spans="1:4" ht="23.25" customHeight="1">
+      <c r="A6" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+    </row>
+    <row r="7" spans="1:4" ht="4.5" customHeight="1" thickBot="1">
+      <c r="B7" s="19"/>
+    </row>
+    <row r="8" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" s="15">
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="13">
         <v>1</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>228</v>
+      <c r="C9" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="7" t="s">
+        <v>218</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>235</v>
+        <v>219</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="7" t="s">
+        <v>222</v>
       </c>
       <c r="B11" s="1">
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>241</v>
+        <v>223</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34">
+      <c r="A12" s="7" t="s">
+        <v>228</v>
       </c>
       <c r="B12" s="1">
         <v>4</v>
       </c>
-      <c r="C12" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>244</v>
+      <c r="C12" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="7" t="s">
+        <v>231</v>
       </c>
       <c r="B13" s="1">
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>247</v>
+        <v>232</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="7" t="s">
+        <v>236</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
+        <v>234</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34">
+      <c r="A15" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="7"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="7"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="7"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="7"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="7"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="10"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="7"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="7"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="7"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="7"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="7"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="10"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="7"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="10"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="7"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="10"/>
-    </row>
-    <row r="28" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="11"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="13"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2114,1077 +2052,1040 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="5.25" customWidth="1"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="16.58203125" customWidth="1"/>
     <col min="3" max="3" width="17.75" customWidth="1"/>
     <col min="4" max="4" width="56" customWidth="1"/>
-    <col min="5" max="5" width="38.125" customWidth="1"/>
-    <col min="6" max="6" width="28.125" customWidth="1"/>
+    <col min="5" max="5" width="38.08203125" customWidth="1"/>
+    <col min="6" max="6" width="28.08203125" customWidth="1"/>
     <col min="7" max="7" width="54" customWidth="1"/>
-    <col min="8" max="8" width="49.125" customWidth="1"/>
+    <col min="8" max="8" width="49.08203125" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
-    <col min="10" max="10" width="11.875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" style="5" customWidth="1"/>
     <col min="11" max="11" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="30">
       <c r="A1" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="21.75" customHeight="1">
+      <c r="B7" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="85">
+      <c r="B8" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J8" s="26">
+        <v>42891</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" ht="68">
+      <c r="B9" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="6" t="s">
+      <c r="E9" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J9" s="26">
+        <v>42891</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" ht="85">
+      <c r="B10" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="24" t="s">
+      <c r="G10" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J10" s="26">
+        <v>42891</v>
+      </c>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" ht="85">
+      <c r="B11" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J11" s="26">
+        <v>42891</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" ht="85">
+      <c r="B12" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J12" s="26">
+        <v>42891</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" ht="102">
+      <c r="B13" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="G9" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J9" s="28">
+      <c r="J13" s="26">
+        <v>42892</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="34">
+      <c r="B14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J14" s="26">
         <v>42891</v>
       </c>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="B10" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J10" s="28">
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" ht="51">
+      <c r="B15" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="J15" s="26">
+        <v>42892</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="85">
+      <c r="B16" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J16" s="26">
         <v>42891</v>
       </c>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B11" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J11" s="28">
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="2:11" ht="68">
+      <c r="B17" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="J17" s="26">
+        <v>42892</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="68">
+      <c r="B18" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J18" s="26">
         <v>42891</v>
       </c>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J12" s="28">
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="2:11" ht="85">
+      <c r="B19" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J19" s="26">
         <v>42891</v>
       </c>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J13" s="28">
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="2:11" ht="34">
+      <c r="B20" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J20" s="26">
         <v>42891</v>
       </c>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" ht="99" x14ac:dyDescent="0.3">
-      <c r="B14" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="J14" s="28">
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="2:11" ht="51">
+      <c r="B21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J21" s="26">
         <v>42891</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B15" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J15" s="28">
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="2:11" ht="34">
+      <c r="B22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J22" s="26">
         <v>42891</v>
       </c>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="B16" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="J16" s="28">
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="2:11" ht="102">
+      <c r="B23" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="J23" s="26">
+        <v>42892</v>
+      </c>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="2:11" ht="135.75" customHeight="1">
+      <c r="B24" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J24" s="26">
         <v>42891</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B17" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J17" s="28">
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="B25" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J25" s="26">
         <v>42891</v>
       </c>
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="2:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="B18" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>233</v>
-      </c>
-      <c r="J18" s="28">
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="2:11">
+      <c r="B26" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J26" s="26">
         <v>42891</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="B19" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J19" s="28">
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="2:11" ht="68">
+      <c r="B27" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="H27" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J27" s="26">
         <v>42891</v>
       </c>
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="2:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B20" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J20" s="28">
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="2:11" ht="33.75" customHeight="1">
+      <c r="B28" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J28" s="26">
         <v>42891</v>
       </c>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="2:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B21" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="H21" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J21" s="28">
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="2:11" ht="51">
+      <c r="B29" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H29" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J29" s="26">
         <v>42891</v>
       </c>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G22" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="H22" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J22" s="28">
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="2:11" ht="51">
+      <c r="B30" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J30" s="26">
         <v>42891</v>
       </c>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="2:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B23" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J23" s="28">
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="2:11" ht="51">
+      <c r="B31" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H31" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J31" s="26">
         <v>42891</v>
       </c>
-      <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="2:11" ht="135.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="C24" s="29" t="s">
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="2:11" ht="51">
+      <c r="B32" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J32" s="26">
+        <v>42891</v>
+      </c>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="2:11" ht="51">
+      <c r="B33" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H33" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J33" s="26">
+        <v>42891</v>
+      </c>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="2:11" ht="51">
+      <c r="B34" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H34" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J34" s="26">
+        <v>42891</v>
+      </c>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="2:11" ht="51">
+      <c r="B35" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="F24" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="I24" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="J24" s="28">
-        <v>42892</v>
-      </c>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
+      <c r="F35" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J35" s="26">
+        <v>42891</v>
+      </c>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="2:11" ht="34">
+      <c r="B36" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="C25" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="C36" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J25" s="28">
+      <c r="I36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J36" s="26">
         <v>42891</v>
       </c>
-      <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B26" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="H26" s="1" t="s">
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="2:11" ht="34">
+      <c r="B37" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J37" s="26">
+        <v>42891</v>
+      </c>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="2:11" ht="34">
+      <c r="B38" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="J26" s="28">
+      <c r="E38" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J38" s="26">
         <v>42891</v>
       </c>
-      <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="J27" s="28">
-        <v>42891</v>
-      </c>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="2:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="24" t="s">
-        <v>217</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G28" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="H28" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="J28" s="28">
-        <v>42891</v>
-      </c>
-      <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="2:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B29" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G29" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="H29" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J29" s="28">
-        <v>42891</v>
-      </c>
-      <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B30" s="24" t="s">
-        <v>218</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H30" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="J30" s="28">
-        <v>42891</v>
-      </c>
-      <c r="K30" s="1"/>
-    </row>
-    <row r="31" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B31" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="H31" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="J31" s="28">
-        <v>42891</v>
-      </c>
-      <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B32" s="24" t="s">
-        <v>220</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>181</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="H32" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J32" s="28">
-        <v>42891</v>
-      </c>
-      <c r="K32" s="1"/>
-    </row>
-    <row r="33" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B33" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="H33" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J33" s="28">
-        <v>42891</v>
-      </c>
-      <c r="K33" s="1"/>
-    </row>
-    <row r="34" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B34" s="24" t="s">
-        <v>222</v>
-      </c>
-      <c r="C34" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="H34" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="J34" s="28">
-        <v>42891</v>
-      </c>
-      <c r="K34" s="1"/>
-    </row>
-    <row r="35" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B35" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="C35" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="H35" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="J35" s="28">
-        <v>42891</v>
-      </c>
-      <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B36" s="24" t="s">
-        <v>225</v>
-      </c>
-      <c r="C36" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J36" s="28">
-        <v>42891</v>
-      </c>
-      <c r="K36" s="1"/>
-    </row>
-    <row r="37" spans="2:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B37" s="24" t="s">
-        <v>224</v>
-      </c>
-      <c r="C37" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G37" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J37" s="28">
-        <v>42891</v>
-      </c>
-      <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="2:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B38" s="24" t="s">
-        <v>226</v>
-      </c>
-      <c r="C38" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="J38" s="28">
-        <v>42891</v>
-      </c>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="2:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B39" s="24" t="s">
-        <v>227</v>
-      </c>
-      <c r="C39" s="30" t="s">
-        <v>184</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="J39" s="28">
-        <v>42891</v>
-      </c>
+    <row r="39" spans="2:11">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="6"/>
       <c r="K39" s="1"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8">
-      <formula1>"Pass,Fail"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
테스트케이스.xlsx TC-0032~TC-0035 결함 Pass로 수정
</commit_message>
<xml_diff>
--- a/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스.xlsx
+++ b/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="280">
   <si>
     <t>TestCase ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1256,12 +1256,29 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Fail</t>
+    <t>2017.06.07</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TC-0032~TC-0035 
 테스트결과 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0032~TC-0035
+결함 Pass로 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정화인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#938</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1980,7 +1997,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1990,8 +2007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -2165,11 +2182,19 @@
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="6"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="7"/>
+    <row r="18" spans="1:4" ht="34">
+      <c r="A18" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="6"/>
@@ -2245,9 +2270,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -2283,7 +2308,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2291,7 +2316,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21.75" customHeight="1">
@@ -2810,7 +2835,9 @@
       <c r="J23" s="25">
         <v>42892</v>
       </c>
-      <c r="K23" s="1"/>
+      <c r="K23" s="1" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="24" spans="2:11" ht="135.75" customHeight="1">
       <c r="B24" s="1" t="s">
@@ -3285,7 +3312,7 @@
         <v>242</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="J39" s="25">
         <v>42893</v>
@@ -3317,7 +3344,7 @@
         <v>259</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>274</v>
+        <v>128</v>
       </c>
       <c r="J40" s="25">
         <v>42893</v>
@@ -3349,7 +3376,7 @@
         <v>260</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>274</v>
+        <v>128</v>
       </c>
       <c r="J41" s="25">
         <v>42893</v>
@@ -3381,7 +3408,7 @@
         <v>261</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>274</v>
+        <v>128</v>
       </c>
       <c r="J42" s="25">
         <v>42893</v>

</xml_diff>